<commit_message>
debugging de precarga A/B
</commit_message>
<xml_diff>
--- a/src/playlistprueba.xlsx
+++ b/src/playlistprueba.xlsx
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>